<commit_message>
planned places for testing targets
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rara8122/Library/Mobile Documents/com~apple~CloudDocs/School/Software Engineering/eclipse-workspace/ClueGame/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2093EAE-536B-A94B-A3DE-ACF3604CD56A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643587FA-E432-6E47-8DA3-09655CABDA9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="100" windowWidth="28560" windowHeight="17900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="45">
   <si>
     <t>X</t>
   </si>
@@ -149,13 +149,34 @@
   </si>
   <si>
     <t>P*</t>
+  </si>
+  <si>
+    <t>Door Direction Tests</t>
+  </si>
+  <si>
+    <t>W&lt;</t>
+  </si>
+  <si>
+    <t>Room Adjacencies</t>
+  </si>
+  <si>
+    <t>Door Adjacencies</t>
+  </si>
+  <si>
+    <t>Walkway Adjacencies</t>
+  </si>
+  <si>
+    <t>Test Targets</t>
+  </si>
+  <si>
+    <t>Test Occupied</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,8 +184,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,6 +252,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC18FFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFF1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -238,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -249,6 +294,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -257,6 +306,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FF00FFF1"/>
+      <color rgb="FFC18FFF"/>
       <color rgb="FFFF2AFF"/>
     </mruColors>
   </colors>
@@ -568,18 +619,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE21"/>
+  <dimension ref="A1:AG21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="31" width="3.6640625" customWidth="1"/>
+    <col min="33" max="33" width="36.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B1">
         <v>0</v>
       </c>
@@ -671,7 +723,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -720,7 +772,7 @@
       <c r="P2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="13" t="s">
         <v>1</v>
       </c>
       <c r="R2" s="5" t="s">
@@ -766,7 +818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -860,8 +912,11 @@
       <c r="AE3" s="5" t="s">
         <v>0</v>
       </c>
+      <c r="AG3" s="11" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -955,8 +1010,11 @@
       <c r="AE4" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="AG4" s="7" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1050,8 +1108,11 @@
       <c r="AE5" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="AG5" s="8" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1145,8 +1206,11 @@
       <c r="AE6" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="AG6" s="9" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1204,7 +1268,7 @@
       <c r="S7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="T7" s="4" t="s">
+      <c r="T7" s="11" t="s">
         <v>14</v>
       </c>
       <c r="U7" s="1" t="s">
@@ -1240,8 +1304,11 @@
       <c r="AE7" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="AG7" s="13" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1335,8 +1402,11 @@
       <c r="AE8" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="AG8" s="12" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1379,7 +1449,7 @@
       <c r="N9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="O9" s="13" t="s">
         <v>1</v>
       </c>
       <c r="P9" s="1" t="s">
@@ -1431,7 +1501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1526,7 +1596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1621,14 +1691,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="11" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -1655,7 +1725,7 @@
       <c r="K12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="L12" s="11" t="s">
         <v>0</v>
       </c>
       <c r="M12" s="3" t="s">
@@ -1676,7 +1746,7 @@
       <c r="R12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="S12" s="13" t="s">
         <v>21</v>
       </c>
       <c r="T12" s="2" t="s">
@@ -1716,7 +1786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1780,8 +1850,8 @@
       <c r="U13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="V13" s="1" t="s">
-        <v>1</v>
+      <c r="V13" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="W13" s="1" t="s">
         <v>1</v>
@@ -1811,7 +1881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1827,7 +1897,7 @@
       <c r="E14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="13" t="s">
         <v>25</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -1878,7 +1948,7 @@
       <c r="V14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="W14" s="4" t="s">
+      <c r="W14" s="13" t="s">
         <v>20</v>
       </c>
       <c r="X14" s="2" t="s">
@@ -1906,7 +1976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2001,7 +2071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2053,7 +2123,7 @@
       <c r="Q16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R16" s="4" t="s">
+      <c r="R16" s="11" t="s">
         <v>27</v>
       </c>
       <c r="S16" s="1" t="s">
@@ -2124,7 +2194,7 @@
       <c r="I17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="8" t="s">
         <v>20</v>
       </c>
       <c r="K17" s="2" t="s">
@@ -2270,7 +2340,7 @@
       <c r="Z18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AA18" s="1" t="s">
+      <c r="AA18" s="11" t="s">
         <v>33</v>
       </c>
       <c r="AB18" s="2" t="s">

</xml_diff>